<commit_message>
Modifiqué las historias de usuario y la descripción de la aplicación. Además, añadí el mockup de la versión web y empecé a desarrollar esta versión en HTML
</commit_message>
<xml_diff>
--- a/historias_plantilla(1).xlsx
+++ b/historias_plantilla(1).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santiago.martinezl\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Desarrollo Web\Proyecto\ProyectoDesarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8BC4EB-CCC8-48DE-8E3A-0C16E9949048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>id</t>
   </si>
@@ -71,12 +66,6 @@
     <t xml:space="preserve">ver fotos </t>
   </si>
   <si>
-    <t>los demas las puedan ver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ver fotos de gatitos </t>
-  </si>
-  <si>
     <t xml:space="preserve">tener una cuenta </t>
   </si>
   <si>
@@ -92,30 +81,12 @@
     <t xml:space="preserve">dar like a fotos </t>
   </si>
   <si>
-    <t xml:space="preserve">los demas puedan ver que le di like </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ver cuantos likes tiene una foto </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pueda saber que fotos son populares </t>
-  </si>
-  <si>
     <t xml:space="preserve">seguir a otros usuarios </t>
   </si>
   <si>
-    <t xml:space="preserve">pueda ver sus fotos en mi pagina de inicio </t>
-  </si>
-  <si>
     <t xml:space="preserve">ser seguido por otros usuarios </t>
   </si>
   <si>
-    <t xml:space="preserve">puedan ver mis fotos en su pagina de inicio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tener una pagina de inicio </t>
-  </si>
-  <si>
     <t xml:space="preserve">pueda ver las fotos de los usuarios que sigo </t>
   </si>
   <si>
@@ -125,79 +96,100 @@
     <t xml:space="preserve">mi cuenta se cierre </t>
   </si>
   <si>
-    <t xml:space="preserve">quiero tener una pestaña de log in </t>
-  </si>
-  <si>
-    <t xml:space="preserve">quiero tener una lista de las personas que sigo </t>
-  </si>
-  <si>
     <t xml:space="preserve">tener un perfil </t>
   </si>
   <si>
-    <t xml:space="preserve">puedan ver mis fotos, seguirme, ver a quien sigo </t>
-  </si>
-  <si>
-    <t>dar click en una foto y poder verla mas grande</t>
-  </si>
-  <si>
     <t xml:space="preserve">pueda ver mejor la foto </t>
   </si>
   <si>
-    <t xml:space="preserve">tener una barra de busqueda </t>
-  </si>
-  <si>
     <t>al dar "buscar " me aparezcan fotos o perfiles relacionados</t>
   </si>
   <si>
-    <t xml:space="preserve">al hacer log in me diriga a mi pagina de inicio </t>
-  </si>
-  <si>
     <t xml:space="preserve">pueda cambiar esa lista y se actualicen los datos </t>
   </si>
   <si>
-    <t xml:space="preserve">saber cuantos likes tengo en total </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ver que tan polular soy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">podre acceder desde mi pc o celular </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sea comodo navegar en cualquiera de ellos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">quiero dar click en un boton </t>
-  </si>
-  <si>
     <t xml:space="preserve">pueda acceder a mi perfil </t>
   </si>
   <si>
     <t xml:space="preserve"> usuario </t>
   </si>
   <si>
-    <t xml:space="preserve">dar click en boton </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pueda ir a mi pagina de inicio </t>
-  </si>
-  <si>
     <t xml:space="preserve"> me indique si tengo notificaciones</t>
   </si>
   <si>
     <t xml:space="preserve">ver una campanita </t>
   </si>
   <si>
-    <t xml:space="preserve">ver cuanos seguidores tengo </t>
-  </si>
-  <si>
     <t xml:space="preserve">esta cantidad aparezca en mi perfil </t>
+  </si>
+  <si>
+    <t>los demás las puedan ver</t>
+  </si>
+  <si>
+    <t>pueda apreciar la ternura de los animales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">los demás puedan ver que le di like </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ver cuántos likes tiene una foto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pueda saber qué fotos son populares </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pueda ver sus fotos en mi página de inicio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">puedan ver mis fotos en su página de inicio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tener una página de inicio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tener una pestaña de log in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">me dirija a mi página de inicio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tener una lista de las personas que sigo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">puedan ver mis fotos, seguirme, ver a quién sigo y quién me sigue </t>
+  </si>
+  <si>
+    <t>dar click en una foto y poder verla más grande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tener una barra de búsqueda </t>
+  </si>
+  <si>
+    <t>saber cuántas publicaciones he realizado</t>
+  </si>
+  <si>
+    <t>la gente y yo podamos ver qué tan activo soy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poder acceder desde mi pc o celular </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sea cómodo navegar en cualquiera de ellos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dar click en un botón </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pueda ir a mi página de inicio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ver cuántos seguidores tengo </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,10 +253,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,25 +570,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" customWidth="1"/>
-    <col min="5" max="5" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" customWidth="1"/>
+    <col min="5" max="5" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -608,16 +600,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
@@ -627,10 +619,10 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -644,7 +636,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F3">
         <v>8</v>
@@ -653,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -667,7 +659,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F4">
         <v>8</v>
@@ -676,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -687,10 +679,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>8</v>
@@ -699,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -710,10 +702,10 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>8</v>
@@ -722,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -733,10 +725,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F7">
         <v>8</v>
@@ -745,7 +737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -756,10 +748,10 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F8">
         <v>8</v>
@@ -768,7 +760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -779,10 +771,10 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -791,7 +783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -802,10 +794,10 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -814,7 +806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -825,10 +817,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F11">
         <v>8</v>
@@ -837,7 +829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -848,10 +840,10 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F12">
         <v>8</v>
@@ -860,7 +852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -871,10 +863,10 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F13">
         <v>8</v>
@@ -883,7 +875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -894,10 +886,10 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="F14">
         <v>8</v>
@@ -906,7 +898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -917,10 +909,10 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F15">
         <v>9</v>
@@ -929,7 +921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -940,10 +932,10 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F16">
         <v>7</v>
@@ -952,7 +944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -963,10 +955,10 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F17">
         <v>7</v>
@@ -975,7 +967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -986,10 +978,10 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F18">
         <v>7</v>
@@ -998,7 +990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1009,10 +1001,10 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -1021,7 +1013,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1032,10 +1024,10 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F20">
         <v>9</v>
@@ -1044,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1052,13 +1044,13 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F21">
         <v>9</v>
@@ -1067,7 +1059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1078,10 +1070,10 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F22">
         <v>7</v>
@@ -1090,7 +1082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1104,7 +1096,7 @@
         <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="F23">
         <v>6</v>
@@ -1113,8 +1105,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>